<commit_message>
raw data collections (thanks odoe)
</commit_message>
<xml_diff>
--- a/EdChoice Data Format.xlsx
+++ b/EdChoice Data Format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdanninger/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdanninger/Documents/GitHub/EdChoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22B0D24E-A663-2E40-984C-4B5360CECB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FC3937-6CDD-8941-8935-0758639E9F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{BBB08C19-94EB-5F42-BB01-6DCC2FB812EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{BBB08C19-94EB-5F42-BB01-6DCC2FB812EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>District Name</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Grade Level</t>
+  </si>
+  <si>
+    <t>AYP Met?</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85950818-F432-5048-91B1-F08D10845CC8}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +481,7 @@
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -520,6 +523,9 @@
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>